<commit_message>
Initial collection based on chromoproteins in the iGEM Registry
</commit_message>
<xml_diff>
--- a/Chromoproteins/Chromoproteins.xlsx
+++ b/Chromoproteins/Chromoproteins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Chromoproteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE45A270-7716-C64A-B704-18D92C83832F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8C1E4-CE85-6248-AE95-52B1BB488D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28160" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7634" uniqueCount="7553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7644" uniqueCount="7556">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22665,9 +22665,6 @@
     <t>Actinia equina</t>
   </si>
   <si>
-    <t>This version is codon optimized for E coli by Bioneer Corp.</t>
-  </si>
-  <si>
     <t>eforRed</t>
   </si>
   <si>
@@ -22710,9 +22707,6 @@
     <t>asPink</t>
   </si>
   <si>
-    <t>This version is codon optimized for E coli by Genscript</t>
-  </si>
-  <si>
     <t>spisPink</t>
   </si>
   <si>
@@ -22762,6 +22756,21 @@
   </si>
   <si>
     <t>Anemonia majano</t>
+  </si>
+  <si>
+    <t>This version is codon optimized for E coli</t>
+  </si>
+  <si>
+    <t>Chromoproteins in vector</t>
+  </si>
+  <si>
+    <t>K864401, K592012, K592011, K592010, K592009, K1033933, K1033932, K1033902, K1033919, K1033916, K1033910, K1033906</t>
+  </si>
+  <si>
+    <t>Chromoprotein Collection</t>
+  </si>
+  <si>
+    <t>Vinoo Selvarajah</t>
   </si>
 </sst>
 </file>
@@ -23158,13 +23167,13 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23622,7 +23631,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23645,7 +23654,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>7554</v>
+      </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -23657,7 +23668,9 @@
       <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>7555</v>
+      </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -23692,12 +23705,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -23887,7 +23900,7 @@
       <c r="I13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="41" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="3" t="s">
@@ -23949,14 +23962,14 @@
         <v>47</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>7520</v>
+        <v>7551</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="47" t="s">
         <v>7517</v>
       </c>
       <c r="H15" s="18" t="s">
@@ -23978,25 +23991,25 @@
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="50" t="s">
-        <v>7521</v>
+      <c r="A16" s="47" t="s">
+        <v>7520</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>7520</v>
+        <v>7551</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="47" t="s">
+        <v>7521</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>7522</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>7523</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>7419</v>
@@ -24015,13 +24028,13 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="41" t="s">
-        <v>7524</v>
+        <v>7523</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>7520</v>
+        <v>7551</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -24029,10 +24042,10 @@
         <v>42</v>
       </c>
       <c r="G17" s="41" t="s">
+        <v>7524</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>7525</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>7526</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>7419</v>
@@ -24051,7 +24064,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="41" t="s">
-        <v>7528</v>
+        <v>7527</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>47</v>
@@ -24063,10 +24076,10 @@
         <v>42</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>7530</v>
+        <v>7529</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>7527</v>
+        <v>7526</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="18" t="b">
@@ -24083,7 +24096,7 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="41" t="s">
-        <v>7529</v>
+        <v>7528</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>47</v>
@@ -24095,10 +24108,10 @@
         <v>42</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>7531</v>
+        <v>7530</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>7527</v>
+        <v>7526</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="18" t="b">
@@ -24115,13 +24128,13 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="41" t="s">
-        <v>7534</v>
+        <v>7533</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>7535</v>
+        <v>7551</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="18"/>
@@ -24129,10 +24142,10 @@
         <v>42</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>7533</v>
+        <v>7532</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>7532</v>
+        <v>7531</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>7419</v>
@@ -24151,13 +24164,13 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="41" t="s">
-        <v>7536</v>
+        <v>7534</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>7535</v>
+        <v>7551</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="18"/>
@@ -24165,10 +24178,10 @@
         <v>42</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>7537</v>
+        <v>7535</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>7419</v>
@@ -24187,13 +24200,13 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="41" t="s">
-        <v>7539</v>
+        <v>7537</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>7535</v>
+        <v>7551</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -24201,10 +24214,10 @@
         <v>42</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>7540</v>
+        <v>7538</v>
       </c>
       <c r="H22" s="41" t="s">
-        <v>7541</v>
+        <v>7539</v>
       </c>
       <c r="I22" s="18" t="s">
         <v>7419</v>
@@ -24223,13 +24236,13 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="41" t="s">
-        <v>7542</v>
+        <v>7540</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>7535</v>
+        <v>7551</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -24237,10 +24250,10 @@
         <v>42</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>7543</v>
+        <v>7541</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>7551</v>
+        <v>7549</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>7419</v>
@@ -24259,13 +24272,13 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="41" t="s">
-        <v>7544</v>
+        <v>7542</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>7535</v>
+        <v>7551</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="18"/>
@@ -24273,10 +24286,10 @@
         <v>42</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>7545</v>
+        <v>7543</v>
       </c>
       <c r="H24" s="41" t="s">
-        <v>7552</v>
+        <v>7550</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>7419</v>
@@ -24295,13 +24308,13 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="41" t="s">
-        <v>7546</v>
+        <v>7544</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>7550</v>
+        <v>7548</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="18"/>
@@ -24309,7 +24322,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>7547</v>
+        <v>7545</v>
       </c>
       <c r="H25" s="41" t="s">
         <v>7417</v>
@@ -24329,13 +24342,13 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="41" t="s">
-        <v>7548</v>
+        <v>7546</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>7550</v>
+        <v>7548</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -24343,7 +24356,7 @@
         <v>42</v>
       </c>
       <c r="G26" s="41" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="H26" s="41" t="s">
         <v>7417</v>
@@ -24362,20 +24375,30 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="41"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="41" t="s">
+        <v>7501</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>53</v>
+      </c>
       <c r="C27" s="18"/>
       <c r="D27" s="20"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="41"/>
+      <c r="F27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>7501</v>
+      </c>
       <c r="H27" s="41"/>
-      <c r="I27" s="18"/>
+      <c r="I27" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J27" s="18" t="b">
         <v>0</v>
       </c>
       <c r="K27" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
@@ -25630,7 +25653,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26123,14 +26146,20 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="A14" s="21"/>
+      <c r="A14" s="47" t="s">
+        <v>7552</v>
+      </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>7501</v>
+      </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="47" t="s">
+        <v>7553</v>
+      </c>
       <c r="H14" s="18"/>
       <c r="I14" s="32"/>
       <c r="J14" s="18"/>
@@ -69306,64 +69335,64 @@
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="48" t="s">
         <v>7519</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="51" t="s">
-        <v>7523</v>
+      <c r="A31" s="48" t="s">
+        <v>7522</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="A32" s="51" t="s">
-        <v>7526</v>
+      <c r="A32" s="48" t="s">
+        <v>7525</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="51" t="s">
-        <v>7527</v>
+      <c r="A33" s="48" t="s">
+        <v>7526</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="51" t="s">
-        <v>7532</v>
+      <c r="A34" s="48" t="s">
+        <v>7531</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35" s="51" t="s">
-        <v>7538</v>
+      <c r="A35" s="48" t="s">
+        <v>7536</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="51" t="s">
-        <v>7541</v>
+      <c r="A36" s="48" t="s">
+        <v>7539</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="51" t="s">
-        <v>7551</v>
+      <c r="A37" s="48" t="s">
+        <v>7549</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A38" s="51" t="s">
-        <v>7552</v>
+      <c r="A38" s="48" t="s">
+        <v>7550</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>

</xml_diff>

<commit_message>
Small fix (changed parts to False for Final Product) which should allow for the pSB1C3 to be viewed as the vector, and added simple description
</commit_message>
<xml_diff>
--- a/Chromoproteins/Chromoproteins.xlsx
+++ b/Chromoproteins/Chromoproteins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Chromoproteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8C1E4-CE85-6248-AE95-52B1BB488D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2307DA4-16E4-1941-9E64-E6C2B991854D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28160" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28160" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7644" uniqueCount="7556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7645" uniqueCount="7557">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22771,6 +22771,9 @@
   </si>
   <si>
     <t>Vinoo Selvarajah</t>
+  </si>
+  <si>
+    <t>A collection of iGEM Registry chromoproteins from Team Uppsala, useful for reporters and projects that require pigments (dyes, bio-art, etc.). This collection should be expanded upon to include chromoproteins outside of the iGEM Registry, particularly newly developed ones.</t>
   </si>
 </sst>
 </file>
@@ -23630,8 +23633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23705,7 +23708,9 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="49"/>
+      <c r="A5" s="49" t="s">
+        <v>7556</v>
+      </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
@@ -23979,7 +23984,7 @@
         <v>7419</v>
       </c>
       <c r="J15" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="18" t="b">
         <v>0</v>
@@ -24015,7 +24020,7 @@
         <v>7419</v>
       </c>
       <c r="J16" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="21" t="b">
         <v>0</v>
@@ -24051,7 +24056,7 @@
         <v>7419</v>
       </c>
       <c r="J17" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="18" t="b">
         <v>0</v>
@@ -24083,7 +24088,7 @@
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="18" t="b">
         <v>0</v>
@@ -24115,7 +24120,7 @@
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="18" t="b">
         <v>0</v>
@@ -24151,7 +24156,7 @@
         <v>7419</v>
       </c>
       <c r="J20" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" s="18" t="b">
         <v>0</v>
@@ -24187,7 +24192,7 @@
         <v>7419</v>
       </c>
       <c r="J21" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="18" t="b">
         <v>0</v>
@@ -24223,7 +24228,7 @@
         <v>7419</v>
       </c>
       <c r="J22" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="18" t="b">
         <v>0</v>
@@ -24259,7 +24264,7 @@
         <v>7419</v>
       </c>
       <c r="J23" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="18" t="b">
         <v>0</v>
@@ -24295,7 +24300,7 @@
         <v>7419</v>
       </c>
       <c r="J24" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="18" t="b">
         <v>0</v>
@@ -24329,7 +24334,7 @@
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="18" t="b">
         <v>0</v>
@@ -24363,7 +24368,7 @@
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="18" t="b">
         <v>0</v>
@@ -25652,8 +25657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
added CDS flanking regions, included pSB1C5.gb (duplicated from Fluor. Reporter Collection), cleared generated files, updated data sources in .xlsx
</commit_message>
<xml_diff>
--- a/Chromoproteins/Chromoproteins.xlsx
+++ b/Chromoproteins/Chromoproteins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Chromoproteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2307DA4-16E4-1941-9E64-E6C2B991854D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB84CF8-6B8B-1E4D-8085-EFBE06D7DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28160" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32580" yWindow="-1880" windowWidth="28160" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7645" uniqueCount="7557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7671" uniqueCount="7576">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22774,6 +22774,63 @@
   </si>
   <si>
     <t>A collection of iGEM Registry chromoproteins from Team Uppsala, useful for reporters and projects that require pigments (dyes, bio-art, etc.). This collection should be expanded upon to include chromoproteins outside of the iGEM Registry, particularly newly developed ones.</t>
+  </si>
+  <si>
+    <t>D1005</t>
+  </si>
+  <si>
+    <t>D1006</t>
+  </si>
+  <si>
+    <t>pSB1C5</t>
+  </si>
+  <si>
+    <t>Includes BsaI and fusion site</t>
+  </si>
+  <si>
+    <t>SynBioHub</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/LmrA/1</t>
+  </si>
+  <si>
+    <t>SynBioHub: https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/LmrA/1</t>
+  </si>
+  <si>
+    <t>{REPLACE_HERE}</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Local Sequence File</t>
+  </si>
+  <si>
+    <t>Local: mRFP1a</t>
+  </si>
+  <si>
+    <t>ExtGB</t>
+  </si>
+  <si>
+    <t>URL for GenBank file</t>
+  </si>
+  <si>
+    <t>https://freegenes.github.io/genbank/BBF10K_003338.gb</t>
+  </si>
+  <si>
+    <t>ExtGB: https://freegenes.github.io/genbank/BBF10K_003338.gb</t>
+  </si>
+  <si>
+    <t>ExtFA</t>
+  </si>
+  <si>
+    <t>URL for FASTA file</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/iGEM-Engineering/iGEM-distribution/develop/scripts/test/test_files/BBa_J23101.fasta</t>
+  </si>
+  <si>
+    <t>ExtFA: http://parts.igem.org/cgi/partsdb/composite_edit/putseq.cgi?part=BBa_J23101</t>
   </si>
 </sst>
 </file>
@@ -23118,7 +23175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23177,6 +23234,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23634,7 +23693,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24381,19 +24440,19 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" s="41" t="s">
-        <v>7501</v>
+        <v>7559</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="20"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>42</v>
+        <v>7566</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>7501</v>
+        <v>7559</v>
       </c>
       <c r="H27" s="41"/>
       <c r="I27" s="18" t="s">
@@ -24412,9 +24471,15 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="41" t="s">
+        <v>7557</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>7560</v>
+      </c>
       <c r="D28" s="20"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
@@ -24434,9 +24499,15 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="41" t="s">
+        <v>7558</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>7560</v>
+      </c>
       <c r="D29" s="20"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
@@ -25658,7 +25729,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26159,14 +26230,18 @@
         <v>1</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>7501</v>
+        <v>7559</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="47" t="s">
+        <v>7557</v>
+      </c>
+      <c r="H14" s="47" t="s">
         <v>7553</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="32"/>
+      <c r="I14" s="32" t="s">
+        <v>7558</v>
+      </c>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -72047,7 +72122,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -72222,36 +72297,84 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="35"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="15" t="s">
+        <v>7561</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>7561</v>
+      </c>
+      <c r="C8" s="52"/>
+      <c r="D8" s="44" t="s">
+        <v>7562</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>7563</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>7564</v>
+      </c>
+      <c r="G8" s="53" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="46"/>
+      <c r="A9" s="15" t="s">
+        <v>7565</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>7566</v>
+      </c>
+      <c r="C9" s="52"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="15" t="s">
+        <v>7567</v>
+      </c>
+      <c r="F9" s="52"/>
+      <c r="G9" s="53" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="G10" s="46"/>
+      <c r="A10" s="15" t="s">
+        <v>7568</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>7569</v>
+      </c>
+      <c r="C10" s="52"/>
+      <c r="D10" s="44" t="s">
+        <v>7570</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>7571</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>7564</v>
+      </c>
+      <c r="G10" s="53" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="46"/>
+      <c r="A11" s="15" t="s">
+        <v>7572</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>7573</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="44" t="s">
+        <v>7574</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>7575</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>7564</v>
+      </c>
+      <c r="G11" s="53" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -75255,6 +75378,12 @@
     <hyperlink ref="D7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
     <hyperlink ref="F7" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
     <hyperlink ref="D3" r:id="rId18" xr:uid="{B834FDED-B3E1-7949-91B7-96E51068AF9E}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{5BB625D8-882C-C143-B723-EFBE69662710}"/>
+    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{2253430C-1FF6-0345-A457-841F9FA0C498}"/>
+    <hyperlink ref="F10" r:id="rId21" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{550E815A-B41A-F947-BB47-18BF0D964D64}"/>
+    <hyperlink ref="F11" r:id="rId22" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{A6254D3D-796E-CD4D-A42F-80A80E3AB09C}"/>
+    <hyperlink ref="D10" r:id="rId23" xr:uid="{5C8EA62C-ED79-D842-A618-35F4B05878DA}"/>
+    <hyperlink ref="D11" r:id="rId24" xr:uid="{B7A141FF-1D60-F84A-A76C-40C3DAE38A80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
added back source id for flanking region parts (D1005-6) no idea how those got erased!
</commit_message>
<xml_diff>
--- a/Chromoproteins/Chromoproteins.xlsx
+++ b/Chromoproteins/Chromoproteins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Chromoproteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB84CF8-6B8B-1E4D-8085-EFBE06D7DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A87B452-8763-0945-8692-9CEF514F8458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32580" yWindow="-1880" windowWidth="28160" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32580" yWindow="-1880" windowWidth="28160" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7671" uniqueCount="7576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7675" uniqueCount="7576">
   <si>
     <t>Collection Name</t>
   </si>
@@ -23229,13 +23229,13 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23692,8 +23692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23767,14 +23767,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="51" t="s">
         <v>7556</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24482,8 +24482,12 @@
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="F28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>7557</v>
+      </c>
       <c r="H28" s="41"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18" t="b">
@@ -24510,8 +24514,12 @@
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="F29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>7558</v>
+      </c>
       <c r="H29" s="41"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18" t="b">
@@ -25728,7 +25736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -72303,17 +72311,17 @@
       <c r="B8" s="15" t="s">
         <v>7561</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="44" t="s">
         <v>7562</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>7563</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="49" t="s">
         <v>7564</v>
       </c>
-      <c r="G8" s="53" t="b">
+      <c r="G8" s="50" t="b">
         <v>1</v>
       </c>
     </row>
@@ -72324,13 +72332,13 @@
       <c r="B9" s="15" t="s">
         <v>7566</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="44"/>
       <c r="E9" s="15" t="s">
         <v>7567</v>
       </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="53" t="b">
+      <c r="F9" s="49"/>
+      <c r="G9" s="50" t="b">
         <v>0</v>
       </c>
     </row>
@@ -72341,17 +72349,17 @@
       <c r="B10" s="15" t="s">
         <v>7569</v>
       </c>
-      <c r="C10" s="52"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="44" t="s">
         <v>7570</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>7571</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="49" t="s">
         <v>7564</v>
       </c>
-      <c r="G10" s="53" t="b">
+      <c r="G10" s="50" t="b">
         <v>1</v>
       </c>
     </row>
@@ -72362,17 +72370,17 @@
       <c r="B11" s="15" t="s">
         <v>7573</v>
       </c>
-      <c r="C11" s="52"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="44" t="s">
         <v>7574</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>7575</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="49" t="s">
         <v>7564</v>
       </c>
-      <c r="G11" s="53" t="b">
+      <c r="G11" s="50" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>